<commit_message>
Up bao cao tuan 8
</commit_message>
<xml_diff>
--- a/Báo cáo tuần 7/BaoCaoCongViec.xlsx
+++ b/Báo cáo tuần 7/BaoCaoCongViec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Git\CNPT_QL_KiTucXa\CNPT_QL_KiTucXa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Git\CNPT_QL_KiTucXa\CNPT_QL_KiTucXa\CNPT_QL_KiTucXa\Báo cáo tuần 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Lê Việt Hoàng</t>
   </si>
@@ -57,13 +57,31 @@
   </si>
   <si>
     <t>Viết Báo Cáo(Word và Excel)</t>
+  </si>
+  <si>
+    <t>Thảo luận công cụ Trello</t>
+  </si>
+  <si>
+    <t>Up file lên Github</t>
+  </si>
+  <si>
+    <t>30 phút</t>
+  </si>
+  <si>
+    <t>15 phút</t>
+  </si>
+  <si>
+    <t>Tìm hiểu viết báo cáo word</t>
+  </si>
+  <si>
+    <t>làm file Excel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +96,48 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -179,42 +232,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -497,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:I8"/>
+      <selection activeCell="D15" sqref="D15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,184 +621,318 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="9"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="4"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="1" t="s">
+      <c r="I5" s="22"/>
+      <c r="J5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="22"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="22"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="2"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="J11:K12"/>
-    <mergeCell ref="H7:I8"/>
-    <mergeCell ref="H9:I10"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="J9:K10"/>
+  <mergeCells count="46">
+    <mergeCell ref="J13:K14"/>
+    <mergeCell ref="J17:K18"/>
+    <mergeCell ref="J19:K20"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="J15:K16"/>
+    <mergeCell ref="F13:G14"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="D19:E20"/>
     <mergeCell ref="D1:K2"/>
     <mergeCell ref="B1:C4"/>
     <mergeCell ref="B7:C8"/>
@@ -714,6 +949,16 @@
     <mergeCell ref="J3:K4"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="H5:I6"/>
+    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="H9:I10"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="J11:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>